<commit_message>
PCQ-181: Updated files to support local CCD build for PCQTEST
</commit_message>
<xml_diff>
--- a/docker/ccd-spreadsheets/PCQ-Example-CaseDefinition.xlsx
+++ b/docker/ccd-spreadsheets/PCQ-Example-CaseDefinition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davejones/Repositories/pcq-consolidation-service/docker/ccd-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE95B0F-AC67-1F4C-9C6C-3D9C16792E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F587536-EB87-D24E-94B8-9B398EE6BE9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33300" windowHeight="15820" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2423,7 +2423,7 @@
     <t>PCQ ID</t>
   </si>
   <si>
-    <t>pcq-test+ccd@gmail.com</t>
+    <t>pcq-scheduler+ccd@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2950,7 +2950,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="277">
+  <cellXfs count="278">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -3658,6 +3658,9 @@
     <xf numFmtId="0" fontId="53" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -3676,256 +3679,6 @@
     <cellStyle name="Normal 2 3" xfId="13" xr:uid="{983C50BB-8B6C-1941-95CA-614B186AEA1E}"/>
   </cellStyles>
   <dxfs count="290">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -5043,6 +4796,256 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -10479,39 +10482,39 @@
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F9" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E16" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E16" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F109" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F109" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10530,40 +10533,40 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="28" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F35" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F35" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F25" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F25" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20977,7 +20980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="219" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -21133,7 +21136,7 @@
       <c r="B8" s="146">
         <v>42736</v>
       </c>
-      <c r="C8" s="192" t="s">
+      <c r="C8" s="277" t="s">
         <v>711</v>
       </c>
       <c r="D8" s="147" t="s">
@@ -24456,8 +24459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD27"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
PCQ-181 Updated to include missing roles script.
</commit_message>
<xml_diff>
--- a/docker/ccd-spreadsheets/PCQ-Example-CaseDefinition.xlsx
+++ b/docker/ccd-spreadsheets/PCQ-Example-CaseDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davejones/Repositories/pcq-consolidation-service/docker/ccd-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F587536-EB87-D24E-94B8-9B398EE6BE9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E51F18-C1A8-9D44-8892-04F7FC67C7FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33300" windowHeight="15820" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4199" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4225" uniqueCount="766">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2417,13 +2417,16 @@
     <t>pcqId</t>
   </si>
   <si>
-    <t>pcq-systemupdate</t>
-  </si>
-  <si>
     <t>PCQ ID</t>
   </si>
   <si>
     <t>pcq-scheduler+ccd@gmail.com</t>
+  </si>
+  <si>
+    <t>caseworker-pcqtest-pcqsystemuser</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -2950,7 +2953,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="278">
+  <cellXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -3658,7 +3661,22 @@
     <xf numFmtId="0" fontId="53" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -12353,8 +12371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D6" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD34"/>
+    <sheetView showGridLines="0" topLeftCell="C2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13718,10 +13736,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Q116"/>
+  <dimension ref="A1:Q119"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="H120" sqref="H120"/>
+    <sheetView showGridLines="0" topLeftCell="E41" zoomScale="193" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18115,7 +18133,7 @@
       <c r="C111" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="D111" s="78" t="s">
+      <c r="D111" s="75" t="s">
         <v>415</v>
       </c>
       <c r="E111" s="78" t="s">
@@ -18340,6 +18358,123 @@
       </c>
       <c r="P116" s="94"/>
       <c r="Q116" s="73"/>
+    </row>
+    <row r="117" spans="1:17" s="18" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="76">
+        <v>42736</v>
+      </c>
+      <c r="B117" s="77"/>
+      <c r="C117" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D117" s="75" t="s">
+        <v>415</v>
+      </c>
+      <c r="E117" s="92" t="s">
+        <v>761</v>
+      </c>
+      <c r="F117" s="130">
+        <v>1</v>
+      </c>
+      <c r="G117" s="277" t="s">
+        <v>619</v>
+      </c>
+      <c r="H117" s="78" t="s">
+        <v>620</v>
+      </c>
+      <c r="I117" s="78" t="s">
+        <v>621</v>
+      </c>
+      <c r="J117" s="93">
+        <v>2</v>
+      </c>
+      <c r="K117" s="94"/>
+      <c r="L117" s="94"/>
+      <c r="M117" s="94"/>
+      <c r="N117" s="94"/>
+      <c r="O117" s="78" t="s">
+        <v>556</v>
+      </c>
+      <c r="P117" s="94"/>
+      <c r="Q117" s="73"/>
+    </row>
+    <row r="118" spans="1:17" s="269" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="279">
+        <v>42736</v>
+      </c>
+      <c r="B118" s="265"/>
+      <c r="C118" s="267" t="s">
+        <v>56</v>
+      </c>
+      <c r="D118" s="267" t="s">
+        <v>416</v>
+      </c>
+      <c r="E118" s="273" t="s">
+        <v>761</v>
+      </c>
+      <c r="F118" s="280">
+        <v>1</v>
+      </c>
+      <c r="G118" s="273" t="s">
+        <v>619</v>
+      </c>
+      <c r="H118" s="267" t="s">
+        <v>620</v>
+      </c>
+      <c r="I118" s="267" t="s">
+        <v>621</v>
+      </c>
+      <c r="J118" s="281">
+        <v>2</v>
+      </c>
+      <c r="K118" s="268"/>
+      <c r="L118" s="268"/>
+      <c r="M118" s="268"/>
+      <c r="N118" s="268"/>
+      <c r="O118" s="267" t="s">
+        <v>556</v>
+      </c>
+      <c r="P118" s="268"/>
+      <c r="Q118" s="282"/>
+    </row>
+    <row r="119" spans="1:17" s="18" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="76">
+        <v>42736</v>
+      </c>
+      <c r="B119" s="77"/>
+      <c r="C119" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D119" s="78" t="s">
+        <v>417</v>
+      </c>
+      <c r="E119" s="92" t="s">
+        <v>761</v>
+      </c>
+      <c r="F119" s="130">
+        <v>1</v>
+      </c>
+      <c r="G119" s="92" t="s">
+        <v>619</v>
+      </c>
+      <c r="H119" s="78" t="s">
+        <v>620</v>
+      </c>
+      <c r="I119" s="78" t="s">
+        <v>621</v>
+      </c>
+      <c r="J119" s="93">
+        <v>1</v>
+      </c>
+      <c r="K119" s="94"/>
+      <c r="L119" s="94"/>
+      <c r="M119" s="94"/>
+      <c r="N119" s="94"/>
+      <c r="O119" s="78" t="s">
+        <v>556</v>
+      </c>
+      <c r="P119" s="94"/>
+      <c r="Q119" s="73"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -20980,8 +21115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="219" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="219" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21136,7 +21271,7 @@
       <c r="B8" s="146">
         <v>42736</v>
       </c>
-      <c r="C8" s="277" t="s">
+      <c r="C8" s="278" t="s">
         <v>711</v>
       </c>
       <c r="D8" s="147" t="s">
@@ -21177,7 +21312,7 @@
         <v>42736</v>
       </c>
       <c r="C10" s="272" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D10" s="271" t="s">
         <v>757</v>
@@ -21217,7 +21352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="188" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
@@ -21492,7 +21627,7 @@
   <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A94" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I106" sqref="I106"/>
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23535,8 +23670,8 @@
       <c r="D113" s="78" t="s">
         <v>761</v>
       </c>
-      <c r="E113" s="94" t="s">
-        <v>762</v>
+      <c r="E113" s="126" t="s">
+        <v>764</v>
       </c>
       <c r="F113" s="78" t="s">
         <v>377</v>
@@ -23558,7 +23693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD87C05-4433-0B47-8359-B17D583CFB7A}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -23678,8 +23813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="170" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24942,7 +25077,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25305,9 +25440,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IN110"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A110" sqref="A110"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -28937,7 +29072,7 @@
         <v>761</v>
       </c>
       <c r="E110" s="274" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F110" s="268"/>
       <c r="G110" s="266" t="s">
@@ -29203,8 +29338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" topLeftCell="A50" zoomScale="190" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -31792,8 +31927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -33082,10 +33217,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C36" zoomScale="194" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -34629,6 +34764,36 @@
       <c r="K50" s="94"/>
       <c r="L50" s="94"/>
     </row>
+    <row r="51" spans="1:12" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="77">
+        <v>42736</v>
+      </c>
+      <c r="B51" s="77"/>
+      <c r="C51" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="78" t="s">
+        <v>478</v>
+      </c>
+      <c r="E51" s="75" t="s">
+        <v>765</v>
+      </c>
+      <c r="F51" s="88" t="s">
+        <v>765</v>
+      </c>
+      <c r="G51" s="89">
+        <v>3</v>
+      </c>
+      <c r="H51" s="92" t="s">
+        <v>761</v>
+      </c>
+      <c r="I51" s="93">
+        <v>1</v>
+      </c>
+      <c r="J51" s="94"/>
+      <c r="K51" s="94"/>
+      <c r="L51" s="94"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
PCQ-181 Update to tweak elastic search.
</commit_message>
<xml_diff>
--- a/docker/ccd-spreadsheets/PCQ-Example-CaseDefinition.xlsx
+++ b/docker/ccd-spreadsheets/PCQ-Example-CaseDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davejones/Repositories/pcq-consolidation-service/docker/ccd-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E51F18-C1A8-9D44-8892-04F7FC67C7FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A2CE94-9530-9346-8BA8-9D613F53D0EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4225" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="766">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2953,7 +2953,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="283">
+  <cellXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -3677,6 +3677,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -18493,10 +18496,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="241" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19216,6 +19219,25 @@
         <v>78</v>
       </c>
       <c r="G36" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="17" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="156">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="156"/>
+      <c r="C37" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="88" t="s">
+        <v>761</v>
+      </c>
+      <c r="E37" s="88"/>
+      <c r="F37" s="88" t="s">
+        <v>762</v>
+      </c>
+      <c r="G37" s="283">
         <v>1</v>
       </c>
     </row>
@@ -25076,8 +25098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25406,7 +25428,7 @@
         <v>42736</v>
       </c>
       <c r="B14" s="39"/>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="41" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="41" t="s">
@@ -33219,7 +33241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C36" zoomScale="194" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C36" zoomScale="194" workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PCQ-181 Update to use correct role.
</commit_message>
<xml_diff>
--- a/docker/ccd-spreadsheets/PCQ-Example-CaseDefinition.xlsx
+++ b/docker/ccd-spreadsheets/PCQ-Example-CaseDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davejones/Repositories/pcq-consolidation-service/docker/ccd-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A2CE94-9530-9346-8BA8-9D613F53D0EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8703A6EE-B239-D040-A999-0ED3D6D96D62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="12" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4235" uniqueCount="766">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2420,13 +2420,13 @@
     <t>PCQ ID</t>
   </si>
   <si>
-    <t>pcq-scheduler+ccd@gmail.com</t>
-  </si>
-  <si>
-    <t>caseworker-pcqtest-pcqsystemuser</t>
-  </si>
-  <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>caseworker-pcqtest-pcqextractor</t>
+  </si>
+  <si>
+    <t>pcq-extractor+ccd@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2953,7 +2953,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="284">
+  <cellXfs count="285">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -3680,6 +3680,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -18498,7 +18501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="241" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="241" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -21137,8 +21140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="219" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="219" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21319,8 +21322,8 @@
       <c r="D9" s="147" t="s">
         <v>757</v>
       </c>
-      <c r="E9" s="147" t="s">
-        <v>27</v>
+      <c r="E9" s="271" t="s">
+        <v>56</v>
       </c>
       <c r="F9" s="147" t="s">
         <v>512</v>
@@ -21334,7 +21337,7 @@
         <v>42736</v>
       </c>
       <c r="C10" s="272" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="D10" s="271" t="s">
         <v>757</v>
@@ -21372,10 +21375,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="188" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView showGridLines="0" zoomScale="188" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21630,6 +21633,21 @@
       </c>
       <c r="E16" s="127" t="s">
         <v>362</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="76">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="94"/>
+      <c r="C17" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="126" t="s">
+        <v>764</v>
+      </c>
+      <c r="E17" s="284" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -21648,7 +21666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A94" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A67" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
@@ -23954,7 +23972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
@@ -24614,10 +24632,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25079,6 +25097,24 @@
         <v>759</v>
       </c>
       <c r="F25" s="127" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="76">
+        <v>42736</v>
+      </c>
+      <c r="B26" s="94"/>
+      <c r="C26" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="78" t="s">
+        <v>512</v>
+      </c>
+      <c r="E26" s="126" t="s">
+        <v>764</v>
+      </c>
+      <c r="F26" s="127" t="s">
         <v>362</v>
       </c>
     </row>
@@ -34798,10 +34834,10 @@
         <v>478</v>
       </c>
       <c r="E51" s="75" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F51" s="88" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="G51" s="89">
         <v>3</v>

</xml_diff>